<commit_message>
Template now handles images that are in root dir of posX dir when cropping.
(E.g. the field will say p1.imageDir='D:\Data_analysis\2014-03-24\pos15\')
</commit_message>
<xml_diff>
--- a/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
+++ b/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="113">
   <si>
     <t>folder name</t>
   </si>
@@ -352,13 +352,16 @@
   </si>
   <si>
     <t>NW_addToSchnitzes_length_test(p1,'onScreen',0);</t>
+  </si>
+  <si>
+    <t>allows pictures in root dir of non-cropped images.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -406,6 +409,13 @@
       <b/>
       <sz val="8"/>
       <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -469,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -505,10 +515,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E149"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -824,10 +835,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1063,10 +1074,10 @@
       <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="24"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
@@ -1085,310 +1096,315 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="str">
+      <c r="A35" s="22" t="str">
+        <f>CONCATENATE("p1.imageDir='",B4,"\",B2,"\",B3,"\'")</f>
+        <v>p1.imageDir='D:\Data_analysis\2014-03-22\pos1\'</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="str">
         <f>CONCATENATE("DJK_cropImages_3colors(p1, ",B$5,", ",B$10,", ",B$11, ", 'cropName', '",B3,"crop');")</f>
         <v>DJK_cropImages_3colors(p1, [2 17 32 47 62 77], [1,1], [1392,1040], 'cropName', 'pos1crop');</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
+      <c r="D36" s="25" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="str">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="str">
         <f>CONCATENATE("p1 = DJK_initschnitz('",B$3,"crop','",B$2,"','e.coli.AMOLF','rootDir','",B$4,"\', 'cropLeftTop', ", B$10,", 'cropRightBottom', ", B$11,",'fluor1','",B$6,"','fluor2','",B$7,"','fluor3','",B$8,"','badseglistname','badseglist');")</f>
         <v>p1 = DJK_initschnitz('pos1crop','2014-03-22','e.coli.AMOLF','rootDir','D:\Data_analysis\', 'cropLeftTop', [1,1], 'cropRightBottom', [1392,1040],'fluor1','none','fluor2','none','fluor3','none','badseglistname','badseglist');</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D40" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="str">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="str">
         <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", B$5, ",'slices', ", B$13, ",'rangeFiltSize', ", B$14, ",'maskMargin', ", B$15, ",'LoG_Smoothing', ", B$16, ",'minCellArea', ", B$17, ",'GaussianFilter', ", B$18, ",'minDepth', ", B$19, ",'neckDepth', ", B$20, ");")</f>
         <v>PN_segmoviephase_3colors(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
       </c>
-      <c r="D40" s="1" t="str">
+      <c r="D41" s="1" t="str">
         <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", E$5, ",'slices', ", E$13, ",'rangeFiltSize', ", E$14, ",'maskMargin', ", E$15, ",'LoG_Smoothing', ", E$16, ",'minCellArea', ", E$17, ",'GaussianFilter', ", E$18, ",'minDepth', ", E$19, ",'neckDepth', ", E$20, ",'medium','rich');")</f>
         <v>PN_segmoviephase_3colors(p1,'segRange', ,'slices', ,'rangeFiltSize', ,'maskMargin', ,'LoG_Smoothing', ,'minCellArea', ,'GaussianFilter', ,'minDepth', ,'neckDepth', ,'medium','rich');</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="str">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="str">
         <f>CONCATENATE("PN_copySegFiles(p1,'segRange', ", B$5, ",'slices', ", B$13, ",'rangeFiltSize', ", B$14, ",'maskMargin', ", B$15, ",'LoG_Smoothing', ", B$16, ",'minCellArea', ", B$17, ",'GaussianFilter', ", B$18, ",'minDepth', ", B$19, ",'neckDepth', ", B$20, ");")</f>
         <v>PN_copySegFiles(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="str">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="str">
         <f>CONCATENATE("MW_manualcheckseg(p1,'manualRange',", B$5, ",'override',1,'assistedCorrection',0);")</f>
         <v>MW_manualcheckseg(p1,'manualRange',[2 17 32 47 62 77],'override',1,'assistedCorrection',0);</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="str">
+    <row r="52" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="str">
         <f>CONCATENATE("DJK_analyzeSeg(p1,'manualRange',", B$5, ");")</f>
         <v>DJK_analyzeSeg(p1,'manualRange',[2 17 32 47 62 77]);</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="4"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="str">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="str">
         <f>CONCATENATE("DJK_trackcomplete(p1,'trackRange',", B$5, ",'trackMethod','singleCell');")</f>
         <v>DJK_trackcomplete(p1,'trackRange',[2 17 32 47 62 77],'trackMethod','singleCell');</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
-    </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
-    </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B60" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="str">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="str">
         <f>CONCATENATE("% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', ", B$5, ",'fluorcolor','fluor1','minimalMode',1);")</f>
         <v>% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', [2 17 32 47 62 77],'fluorcolor','fluor1','minimalMode',1);</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B64" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="4"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="4"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="14" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B70" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
-    </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B72" s="4"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="B73" s="4"/>
-      <c r="C73" s="24" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B74" s="4"/>
+      <c r="C74" s="23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="B75" s="4"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="23"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="B80" s="24"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="7"/>
-    </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="7"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="str">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitLength',[5 80]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 80]);</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="str">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitLength',[100 1000]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[100 1000]);</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="str">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitLength',[5 1000]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 1000]);</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="4"/>
-    </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="str">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitTime',[0 200]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitTime',[0 200]);</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="4"/>
-    </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="str">
+      <c r="B89" s="4"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', ", B$22, ", 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', [0 1000], 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B89" s="4"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="4"/>
-      <c r="B90" s="3"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="4"/>
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="str">
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', ", B$22, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="4"/>
       <c r="B93" s="3"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="4"/>
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B94" s="4"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="str">
+      <c r="B95" s="4"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', ", B$22, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
       <c r="B96" s="3"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1400,11 +1416,11 @@
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="8"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="3"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
+      <c r="A100" s="8"/>
       <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1448,11 +1464,11 @@
       <c r="B110" s="4"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="8"/>
+      <c r="A111" s="4"/>
       <c r="B111" s="4"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="4"/>
+      <c r="A112" s="8"/>
       <c r="B112" s="4"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -1496,16 +1512,16 @@
       <c r="B122" s="4"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="8"/>
+      <c r="A123" s="4"/>
       <c r="B123" s="4"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="3"/>
-      <c r="B124" s="8"/>
+      <c r="A124" s="8"/>
+      <c r="B124" s="4"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
+      <c r="A125" s="3"/>
+      <c r="B125" s="8"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
@@ -1560,15 +1576,15 @@
       <c r="B138" s="4"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="8"/>
+      <c r="A139" s="4"/>
       <c r="B139" s="4"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="3"/>
+      <c r="A140" s="8"/>
       <c r="B140" s="4"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="4"/>
+      <c r="A141" s="3"/>
       <c r="B141" s="4"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -1602,12 +1618,16 @@
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1632,10 +1652,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1783,10 +1803,10 @@
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
@@ -1937,10 +1957,10 @@
       <c r="A55" s="7"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="23"/>
+      <c r="B56" s="24"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
@@ -2014,14 +2034,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">

</xml_diff>

<commit_message>
Minor edit - added title.
</commit_message>
<xml_diff>
--- a/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
+++ b/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="114">
   <si>
     <t>folder name</t>
   </si>
@@ -355,13 +355,16 @@
   </si>
   <si>
     <t>allows pictures in root dir of non-cropped images.</t>
+  </si>
+  <si>
+    <t>FAST ANALYSIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -416,6 +419,11 @@
       <b/>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -479,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -516,10 +524,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -834,171 +843,168 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:5" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+      <c r="A1" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="5"/>
+      <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>97</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>105</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>73</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>84</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="5">
-        <v>35</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="5">
-        <v>20</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="16">
-        <v>250</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>87</v>
+        <v>66</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="5">
-        <v>5</v>
+        <v>67</v>
+      </c>
+      <c r="B18" s="16">
+        <v>250</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="5">
         <v>5</v>
@@ -1006,30 +1012,34 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B21" s="5">
         <v>2</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
@@ -1040,375 +1050,375 @@
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="A26" s="2"/>
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="5">
-        <v>15</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="B28" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="5"/>
-    </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="24"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="B32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="str">
-        <f>CONCATENATE("p1 = DJK_initschnitz('",B$3,"','",B$2,"','e.coli.amolf','rootDir','",B$4,"\', 'cropLeftTop',",B$10,", 'cropRightBottom',",B$11,",'fluor1','",B$6,"','fluor2','",B$7,"','fluor3','",B$8,"');")</f>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="str">
+        <f>CONCATENATE("p1 = DJK_initschnitz('",B$4,"','",B$3,"','e.coli.amolf','rootDir','",B$5,"\', 'cropLeftTop',",B$11,", 'cropRightBottom',",B$12,",'fluor1','",B$7,"','fluor2','",B$8,"','fluor3','",B$9,"');")</f>
         <v>p1 = DJK_initschnitz('pos1','2014-03-22','e.coli.amolf','rootDir','D:\Data_analysis\', 'cropLeftTop',[1,1], 'cropRightBottom',[1392,1040],'fluor1','none','fluor2','none','fluor3','none');</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="str">
-        <f>CONCATENATE("p1.imageDir='",B4,"\",B2,"\",B3,"\'")</f>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="str">
+        <f>CONCATENATE("p1.imageDir='",B5,"\",B3,"\",B4,"\'")</f>
         <v>p1.imageDir='D:\Data_analysis\2014-03-22\pos1\'</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="str">
-        <f>CONCATENATE("DJK_cropImages_3colors(p1, ",B$5,", ",B$10,", ",B$11, ", 'cropName', '",B3,"crop');")</f>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="str">
+        <f>CONCATENATE("DJK_cropImages_3colors(p1, ",B$6,", ",B$11,", ",B$12, ", 'cropName', '",B4,"crop');")</f>
         <v>DJK_cropImages_3colors(p1, [2 17 32 47 62 77], [1,1], [1392,1040], 'cropName', 'pos1crop');</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D37" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="str">
-        <f>CONCATENATE("p1 = DJK_initschnitz('",B$3,"crop','",B$2,"','e.coli.AMOLF','rootDir','",B$4,"\', 'cropLeftTop', ", B$10,", 'cropRightBottom', ", B$11,",'fluor1','",B$6,"','fluor2','",B$7,"','fluor3','",B$8,"','badseglistname','badseglist');")</f>
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="str">
+        <f>CONCATENATE("p1 = DJK_initschnitz('",B$4,"crop','",B$3,"','e.coli.AMOLF','rootDir','",B$5,"\', 'cropLeftTop', ", B$11,", 'cropRightBottom', ", B$12,",'fluor1','",B$7,"','fluor2','",B$8,"','fluor3','",B$9,"','badseglistname','badseglist');")</f>
         <v>p1 = DJK_initschnitz('pos1crop','2014-03-22','e.coli.AMOLF','rootDir','D:\Data_analysis\', 'cropLeftTop', [1,1], 'cropRightBottom', [1392,1040],'fluor1','none','fluor2','none','fluor3','none','badseglistname','badseglist');</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D41" s="17" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="str">
-        <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", B$5, ",'slices', ", B$13, ",'rangeFiltSize', ", B$14, ",'maskMargin', ", B$15, ",'LoG_Smoothing', ", B$16, ",'minCellArea', ", B$17, ",'GaussianFilter', ", B$18, ",'minDepth', ", B$19, ",'neckDepth', ", B$20, ");")</f>
-        <v>PN_segmoviephase_3colors(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
-      </c>
-      <c r="D41" s="1" t="str">
-        <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", E$5, ",'slices', ", E$13, ",'rangeFiltSize', ", E$14, ",'maskMargin', ", E$15, ",'LoG_Smoothing', ", E$16, ",'minCellArea', ", E$17, ",'GaussianFilter', ", E$18, ",'minDepth', ", E$19, ",'neckDepth', ", E$20, ",'medium','rich');")</f>
-        <v>PN_segmoviephase_3colors(p1,'segRange', ,'slices', ,'rangeFiltSize', ,'maskMargin', ,'LoG_Smoothing', ,'minCellArea', ,'GaussianFilter', ,'minDepth', ,'neckDepth', ,'medium','rich');</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="str">
-        <f>CONCATENATE("PN_copySegFiles(p1,'segRange', ", B$5, ",'slices', ", B$13, ",'rangeFiltSize', ", B$14, ",'maskMargin', ", B$15, ",'LoG_Smoothing', ", B$16, ",'minCellArea', ", B$17, ",'GaussianFilter', ", B$18, ",'minDepth', ", B$19, ",'neckDepth', ", B$20, ");")</f>
+        <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", B$6, ",'slices', ", B$14, ",'rangeFiltSize', ", B$15, ",'maskMargin', ", B$16, ",'LoG_Smoothing', ", B$17, ",'minCellArea', ", B$18, ",'GaussianFilter', ", B$19, ",'minDepth', ", B$20, ",'neckDepth', ", B$21, ");")</f>
+        <v>PN_segmoviephase_3colors(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", E$6, ",'slices', ", E$14, ",'rangeFiltSize', ", E$15, ",'maskMargin', ", E$16, ",'LoG_Smoothing', ", E$17, ",'minCellArea', ", E$18, ",'GaussianFilter', ", E$19, ",'minDepth', ", E$20, ",'neckDepth', ", E$21, ",'medium','rich');")</f>
+        <v>PN_segmoviephase_3colors(p1,'segRange', ,'slices', ,'rangeFiltSize', ,'maskMargin', ,'LoG_Smoothing', ,'minCellArea', ,'GaussianFilter', ,'minDepth', ,'neckDepth', ,'medium','rich');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="str">
+        <f>CONCATENATE("PN_copySegFiles(p1,'segRange', ", B$6, ",'slices', ", B$14, ",'rangeFiltSize', ", B$15, ",'maskMargin', ", B$16, ",'LoG_Smoothing', ", B$17, ",'minCellArea', ", B$18, ",'GaussianFilter', ", B$19, ",'minDepth', ", B$20, ",'neckDepth', ", B$21, ");")</f>
         <v>PN_copySegFiles(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="str">
-        <f>CONCATENATE("MW_manualcheckseg(p1,'manualRange',", B$5, ",'override',1,'assistedCorrection',0);")</f>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="str">
+        <f>CONCATENATE("MW_manualcheckseg(p1,'manualRange',", B$6, ",'override',1,'assistedCorrection',0);")</f>
         <v>MW_manualcheckseg(p1,'manualRange',[2 17 32 47 62 77],'override',1,'assistedCorrection',0);</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="str">
-        <f>CONCATENATE("DJK_analyzeSeg(p1,'manualRange',", B$5, ");")</f>
+    <row r="53" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="str">
+        <f>CONCATENATE("DJK_analyzeSeg(p1,'manualRange',", B$6, ");")</f>
         <v>DJK_analyzeSeg(p1,'manualRange',[2 17 32 47 62 77]);</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="str">
-        <f>CONCATENATE("DJK_trackcomplete(p1,'trackRange',", B$5, ",'trackMethod','singleCell');")</f>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="str">
+        <f>CONCATENATE("DJK_trackcomplete(p1,'trackRange',", B$6, ",'trackMethod','singleCell');")</f>
         <v>DJK_trackcomplete(p1,'trackRange',[2 17 32 47 62 77],'trackMethod','singleCell');</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-    </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
-    </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B61" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="4"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
+      <c r="C61" s="4"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="str">
-        <f>CONCATENATE("% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', ", B$5, ",'fluorcolor','fluor1','minimalMode',1);")</f>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="str">
+        <f>CONCATENATE("% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', ", B$6, ",'fluorcolor','fluor1','minimalMode',1);")</f>
         <v>% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', [2 17 32 47 62 77],'fluorcolor','fluor1','minimalMode',1);</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B65" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="4"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="14" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B71" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="4"/>
-    </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="4"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="B74" s="4"/>
-      <c r="C74" s="23" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B75" s="4"/>
+      <c r="C75" s="23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" s="4"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="B76" s="4"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B78" s="4"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="24" t="s">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="24"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="B81" s="25"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="7"/>
-    </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="7"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitLength',[5 80]);")</f>
-        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 80]);</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitLength',[100 1000]);")</f>
-        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[100 1000]);</v>
+        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 80]);")</f>
+        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 80]);</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitLength',[5 1000]);")</f>
+        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[100 1000]);")</f>
+        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[100 1000]);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="str">
+        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 1000]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 1000]);</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
-    </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$22, ", 'onScreen', 0,'fitTime',[0 200]);")</f>
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="str">
+        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitTime',[0 200]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitTime',[0 200]);</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B89" s="4"/>
-    </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="str">
-        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', ", B$22, ", 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);")</f>
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="str">
+        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', ", B$23, ", 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', [0 1000], 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B90" s="4"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="4"/>
-      <c r="B91" s="3"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="4"/>
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="str">
-        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', ", B$22, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="str">
+        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
       <c r="B94" s="3"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="4"/>
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="4"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="str">
-        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', ", B$22, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
+      <c r="B96" s="4"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="str">
+        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
       <c r="B97" s="3"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1420,11 +1430,11 @@
       <c r="B99" s="3"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="8"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="4"/>
+      <c r="A101" s="8"/>
       <c r="B101" s="4"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -1468,11 +1478,11 @@
       <c r="B111" s="4"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="8"/>
+      <c r="A112" s="4"/>
       <c r="B112" s="4"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="4"/>
+      <c r="A113" s="8"/>
       <c r="B113" s="4"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -1516,16 +1526,16 @@
       <c r="B123" s="4"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="8"/>
+      <c r="A124" s="4"/>
       <c r="B124" s="4"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="3"/>
-      <c r="B125" s="8"/>
+      <c r="A125" s="8"/>
+      <c r="B125" s="4"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4"/>
+      <c r="A126" s="3"/>
+      <c r="B126" s="8"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
@@ -1580,15 +1590,15 @@
       <c r="B139" s="4"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="8"/>
+      <c r="A140" s="4"/>
       <c r="B140" s="4"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="3"/>
+      <c r="A141" s="8"/>
       <c r="B141" s="4"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="4"/>
+      <c r="A142" s="3"/>
       <c r="B142" s="4"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -1623,11 +1633,15 @@
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
     </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A81:B81"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1652,10 +1666,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1803,10 +1817,10 @@
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="25"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
@@ -1957,10 +1971,10 @@
       <c r="A55" s="7"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="24"/>
+      <c r="B56" s="25"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
@@ -2034,14 +2048,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">

</xml_diff>

<commit_message>
Microns per pxl is different for the two microscopes, so this needs to be set.
</commit_message>
<xml_diff>
--- a/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
+++ b/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="240" windowWidth="15135" windowHeight="9180"/>
+    <workbookView xWindow="120" yWindow="300" windowWidth="15135" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="pos5_B" sheetId="61" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="117">
   <si>
     <t>folder name</t>
   </si>
@@ -358,6 +358,15 @@
   </si>
   <si>
     <t>FAST ANALYSIS</t>
+  </si>
+  <si>
+    <t>%p.micronsPerPixel = 0.0431;</t>
+  </si>
+  <si>
+    <t>% Only for Tans2 microscope</t>
+  </si>
+  <si>
+    <t>% Only for Tans2 microscope - Note that MetaData dir needs to be in root pos dir.</t>
   </si>
 </sst>
 </file>
@@ -525,10 +534,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -843,16 +852,16 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+      <c r="A1" s="25" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1088,10 +1097,10 @@
       <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="25"/>
+      <c r="B32" s="26"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
@@ -1108,321 +1117,328 @@
       <c r="A35" s="22" t="s">
         <v>106</v>
       </c>
+      <c r="C35" s="22" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="str">
+      <c r="A36" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="22" t="str">
         <f>CONCATENATE("p1.imageDir='",B5,"\",B3,"\",B4,"\'")</f>
         <v>p1.imageDir='D:\Data_analysis\2014-03-22\pos1\'</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="str">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="str">
         <f>CONCATENATE("DJK_cropImages_3colors(p1, ",B$6,", ",B$11,", ",B$12, ", 'cropName', '",B4,"crop');")</f>
         <v>DJK_cropImages_3colors(p1, [2 17 32 47 62 77], [1,1], [1392,1040], 'cropName', 'pos1crop');</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D38" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-    </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="str">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="str">
         <f>CONCATENATE("p1 = DJK_initschnitz('",B$4,"crop','",B$3,"','e.coli.AMOLF','rootDir','",B$5,"\', 'cropLeftTop', ", B$11,", 'cropRightBottom', ", B$12,",'fluor1','",B$7,"','fluor2','",B$8,"','fluor3','",B$9,"','badseglistname','badseglist');")</f>
         <v>p1 = DJK_initschnitz('pos1crop','2014-03-22','e.coli.AMOLF','rootDir','D:\Data_analysis\', 'cropLeftTop', [1,1], 'cropRightBottom', [1392,1040],'fluor1','none','fluor2','none','fluor3','none','badseglistname','badseglist');</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D42" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="str">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="str">
         <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", B$6, ",'slices', ", B$14, ",'rangeFiltSize', ", B$15, ",'maskMargin', ", B$16, ",'LoG_Smoothing', ", B$17, ",'minCellArea', ", B$18, ",'GaussianFilter', ", B$19, ",'minDepth', ", B$20, ",'neckDepth', ", B$21, ");")</f>
         <v>PN_segmoviephase_3colors(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
       </c>
-      <c r="D42" s="1" t="str">
+      <c r="D43" s="1" t="str">
         <f>CONCATENATE("PN_segmoviephase_3colors(p1,'segRange', ", E$6, ",'slices', ", E$14, ",'rangeFiltSize', ", E$15, ",'maskMargin', ", E$16, ",'LoG_Smoothing', ", E$17, ",'minCellArea', ", E$18, ",'GaussianFilter', ", E$19, ",'minDepth', ", E$20, ",'neckDepth', ", E$21, ",'medium','rich');")</f>
         <v>PN_segmoviephase_3colors(p1,'segRange', ,'slices', ,'rangeFiltSize', ,'maskMargin', ,'LoG_Smoothing', ,'minCellArea', ,'GaussianFilter', ,'minDepth', ,'neckDepth', ,'medium','rich');</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="str">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="str">
         <f>CONCATENATE("PN_copySegFiles(p1,'segRange', ", B$6, ",'slices', ", B$14, ",'rangeFiltSize', ", B$15, ",'maskMargin', ", B$16, ",'LoG_Smoothing', ", B$17, ",'minCellArea', ", B$18, ",'GaussianFilter', ", B$19, ",'minDepth', ", B$20, ",'neckDepth', ", B$21, ");")</f>
         <v>PN_copySegFiles(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="str">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="str">
         <f>CONCATENATE("MW_manualcheckseg(p1,'manualRange',", B$6, ",'override',1,'assistedCorrection',0);")</f>
         <v>MW_manualcheckseg(p1,'manualRange',[2 17 32 47 62 77],'override',1,'assistedCorrection',0);</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="str">
+    <row r="54" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="str">
         <f>CONCATENATE("DJK_analyzeSeg(p1,'manualRange',", B$6, ");")</f>
         <v>DJK_analyzeSeg(p1,'manualRange',[2 17 32 47 62 77]);</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="str">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="str">
         <f>CONCATENATE("DJK_trackcomplete(p1,'trackRange',", B$6, ",'trackMethod','singleCell');")</f>
         <v>DJK_trackcomplete(p1,'trackRange',[2 17 32 47 62 77],'trackMethod','singleCell');</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
-    </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
-    </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B62" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
+      <c r="C62" s="4"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="str">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="str">
         <f>CONCATENATE("% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', ", B$6, ",'fluorcolor','fluor1','minimalMode',1);")</f>
         <v>% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', [2 17 32 47 62 77],'fluorcolor','fluor1','minimalMode',1);</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B66" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="14" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B72" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
-    </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B74" s="4"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="B75" s="4"/>
-      <c r="C75" s="23" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B76" s="4"/>
+      <c r="C76" s="23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B79" s="4"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="25" t="s">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="25"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+      <c r="B82" s="26"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="7"/>
-    </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="7"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="str">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 80]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 80]);</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="str">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[100 1000]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[100 1000]);</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="str">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 1000]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 1000]);</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="4"/>
-    </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="str">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitTime',[0 200]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitTime',[0 200]);</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B90" s="4"/>
-    </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="str">
+      <c r="B91" s="4"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', ", B$23, ", 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', [0 1000], 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B91" s="4"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="4"/>
-      <c r="B92" s="3"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="4"/>
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="str">
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="4"/>
       <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="4"/>
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="4"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="str">
+      <c r="B97" s="4"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="4"/>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -1434,11 +1450,11 @@
       <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="8"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="3"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
+      <c r="A102" s="8"/>
       <c r="B102" s="4"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -1482,11 +1498,11 @@
       <c r="B112" s="4"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="8"/>
+      <c r="A113" s="4"/>
       <c r="B113" s="4"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="4"/>
+      <c r="A114" s="8"/>
       <c r="B114" s="4"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -1530,16 +1546,16 @@
       <c r="B124" s="4"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="8"/>
+      <c r="A125" s="4"/>
       <c r="B125" s="4"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="3"/>
-      <c r="B126" s="8"/>
+      <c r="A126" s="8"/>
+      <c r="B126" s="4"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
+      <c r="A127" s="3"/>
+      <c r="B127" s="8"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
@@ -1594,15 +1610,15 @@
       <c r="B140" s="4"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="8"/>
+      <c r="A141" s="4"/>
       <c r="B141" s="4"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="3"/>
+      <c r="A142" s="8"/>
       <c r="B142" s="4"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="4"/>
+      <c r="A143" s="3"/>
       <c r="B143" s="4"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -1636,12 +1652,16 @@
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1666,10 +1686,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1817,10 +1837,10 @@
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="25"/>
+      <c r="B22" s="26"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
@@ -1971,10 +1991,10 @@
       <c r="A55" s="7"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="26"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
@@ -2048,14 +2068,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">

</xml_diff>

<commit_message>
Some additional overhead files.
</commit_message>
<xml_diff>
--- a/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
+++ b/MWtemplate_MW_NWDE_schnitzcell_preliminaryAnalysis_2014-03-23_posX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="300" windowWidth="15135" windowHeight="9120"/>
+    <workbookView xWindow="120" yWindow="360" windowWidth="15135" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="pos5_B" sheetId="61" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="118">
   <si>
     <t>folder name</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>% Only for Tans2 microscope - Note that MetaData dir needs to be in root pos dir.</t>
+  </si>
+  <si>
+    <t>% segmentation without cropping (use when artefacts are present):</t>
   </si>
 </sst>
 </file>
@@ -839,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1173,256 +1176,260 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="str">
+        <f>CONCATENATE("%NW_nocut_segmoviephase_3colors_diffStrains(p1,'segRange', ", B$6, ",'slices', ", B$14, ",'rangeFiltSize', ", B$15, ",'maskMargin', ", B$16, ",'LoG_Smoothing', ", B$17, ",'minCellArea', ", B$18, ",'GaussianFilter', ", B$19, ",'minDepth', ", B$20, ",'neckDepth', ", B$21, ");")</f>
+        <v>%NW_nocut_segmoviephase_3colors_diffStrains(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="str">
         <f>CONCATENATE("PN_copySegFiles(p1,'segRange', ", B$6, ",'slices', ", B$14, ",'rangeFiltSize', ", B$15, ",'maskMargin', ", B$16, ",'LoG_Smoothing', ", B$17, ",'minCellArea', ", B$18, ",'GaussianFilter', ", B$19, ",'minDepth', ", B$20, ",'neckDepth', ", B$21, ");")</f>
         <v>PN_copySegFiles(p1,'segRange', [2 17 32 47 62 77],'slices', [1 2 3],'rangeFiltSize', 35,'maskMargin', 20,'LoG_Smoothing', 2,'minCellArea', 250,'GaussianFilter', 5,'minDepth', 5,'neckDepth', 2);</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="str">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="str">
         <f>CONCATENATE("MW_manualcheckseg(p1,'manualRange',", B$6, ",'override',1,'assistedCorrection',0);")</f>
         <v>MW_manualcheckseg(p1,'manualRange',[2 17 32 47 62 77],'override',1,'assistedCorrection',0);</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="str">
+    <row r="55" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="str">
         <f>CONCATENATE("DJK_analyzeSeg(p1,'manualRange',", B$6, ");")</f>
         <v>DJK_analyzeSeg(p1,'manualRange',[2 17 32 47 62 77]);</v>
       </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="str">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="str">
         <f>CONCATENATE("DJK_trackcomplete(p1,'trackRange',", B$6, ",'trackMethod','singleCell');")</f>
         <v>DJK_trackcomplete(p1,'trackRange',[2 17 32 47 62 77],'trackMethod','singleCell');</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
-    </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
-    </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B63" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="4"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="str">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="str">
         <f>CONCATENATE("% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', ", B$6, ",'fluorcolor','fluor1','minimalMode',1);")</f>
         <v>% DJK_analyzeFluorBackground_anycolor(p1,'manualRange', [2 17 32 47 62 77],'fluorcolor','fluor1','minimalMode',1);</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B67" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="8" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C69" s="4"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="14" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B73" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
-    </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="4"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="B76" s="4"/>
-      <c r="C76" s="23" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B77" s="4"/>
+      <c r="C77" s="23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="4"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="B78" s="4"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="4"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B80" s="4"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="26" t="s">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="26"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+      <c r="B83" s="26"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="7"/>
-    </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="7"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="8" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 80]);")</f>
-        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 80]);</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[100 1000]);")</f>
-        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[100 1000]);</v>
+        <f>CONCATENATE("%fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 80]);")</f>
+        <v>%fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 80]);</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="str">
-        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 1000]);")</f>
-        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 1000]);</v>
+        <f>CONCATENATE("%fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[100 1000]);")</f>
+        <v>%fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[100 1000]);</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="4"/>
+      <c r="A89" s="4" t="str">
+        <f>CONCATENATE("%fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitLength',[5 1000]);")</f>
+        <v>%fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitLength',[5 1000]);</v>
+      </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="str">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="str">
         <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitTime',[0 200]);")</f>
         <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitTime',[0 200]);</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="4"/>
-    </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="str">
+        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitTime',[0 400]);")</f>
+        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitTime',[0 400]);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="str">
+        <f>CONCATENATE("fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', ", B$23, ", 'onScreen', 0,'fitTime',[50 500]);")</f>
+        <v>fitTime = DJK_analyzeMu(p1, schnitzcells, 'xlim', [0 1000], 'onScreen', 0,'fitTime',[50 500]);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="4"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="str">
         <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', ", B$23, ", 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);")</f>
         <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'av_mu_fitNew', 'xlim', [0 1000], 'ylim', [0 1.0], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
-      <c r="B92" s="4"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="4"/>
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="str">
-        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
-        <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
-      </c>
-      <c r="B95" s="3"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
@@ -1430,14 +1437,14 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B97" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="B97" s="3"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="str">
-        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
-        <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
+        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
+        <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G6_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
       </c>
       <c r="B98" s="3"/>
     </row>
@@ -1446,27 +1453,32 @@
       <c r="B99" s="3"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
-      <c r="B100" s="3"/>
+      <c r="A100" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="4"/>
+      <c r="A101" s="4" t="str">
+        <f>CONCATENATE("DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', ", B$23, ", 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);")</f>
+        <v>DJK_plot_avColonyOverTime(p1, schnitzcells, 'G5_mean_all', 'xlim', [0 1000], 'ylim', [0 500], 'fitTime', fitTime, 'onScreen', 0);</v>
+      </c>
       <c r="B101" s="3"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="8"/>
-      <c r="B102" s="4"/>
+      <c r="A102" s="4"/>
+      <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
+      <c r="B103" s="3"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
+      <c r="B104" s="3"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="4"/>
+      <c r="A105" s="8"/>
       <c r="B105" s="4"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -1502,7 +1514,7 @@
       <c r="B113" s="4"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="8"/>
+      <c r="A114" s="4"/>
       <c r="B114" s="4"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -1514,7 +1526,7 @@
       <c r="B116" s="4"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="4"/>
+      <c r="A117" s="8"/>
       <c r="B117" s="4"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -1550,24 +1562,24 @@
       <c r="B125" s="4"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="8"/>
+      <c r="A126" s="4"/>
       <c r="B126" s="4"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="3"/>
-      <c r="B127" s="8"/>
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="4"/>
+      <c r="A129" s="8"/>
       <c r="B129" s="4"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4"/>
+      <c r="A130" s="3"/>
+      <c r="B130" s="8"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
@@ -1614,11 +1626,11 @@
       <c r="B141" s="4"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="8"/>
+      <c r="A142" s="4"/>
       <c r="B142" s="4"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="3"/>
+      <c r="A143" s="4"/>
       <c r="B143" s="4"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -1626,11 +1638,11 @@
       <c r="B144" s="4"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="4"/>
+      <c r="A145" s="8"/>
       <c r="B145" s="4"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="4"/>
+      <c r="A146" s="3"/>
       <c r="B146" s="4"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
@@ -1656,12 +1668,24 @@
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>